<commit_message>
3D models added (template)
</commit_message>
<xml_diff>
--- a/3DayCabLayout.xlsx
+++ b/3DayCabLayout.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C77384-D091-489F-AA74-4579B85ADA7A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A896AE9-1322-4981-8344-5BDC72AE78CC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="702" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -758,7 +758,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9:L9"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U12" sqref="T10:U12"/>
+      <selection activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2187,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>